<commit_message>
[subset_sum] regenerated xlsx and plots
</commit_message>
<xml_diff>
--- a/subset_sum.xlsx
+++ b/subset_sum.xlsx
@@ -11731,10 +11731,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$151:$Z$151</c:f>
+              <c:f>precision!$B$151:$AE$151</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>0.001772075</c:v>
                 </c:pt>
@@ -11809,6 +11809,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>6.408075e-05</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.95206798</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.82414</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.295575</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.7562</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.6907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11825,10 +11840,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$152:$Z$152</c:f>
+              <c:f>precision!$B$152:$AE$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-3.89999999999982e-06</c:v>
                 </c:pt>
@@ -11903,6 +11918,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-0.002109852</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11392587</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.5116</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.965025</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.36950000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.14737499999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11919,10 +11949,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$153:$Z$153</c:f>
+              <c:f>precision!$B$153:$AE$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-0.330597575</c:v>
                 </c:pt>
@@ -11997,6 +12027,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.00013502525</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1531690975</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19.1986625</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19.1352</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19.506425</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.6153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12165,10 +12210,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$155:$Z$155</c:f>
+              <c:f>precision!$B$155:$AE$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-3.284703875</c:v>
                 </c:pt>
@@ -12243,6 +12288,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.20550563</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10885561</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.5940925</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.38935</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.5735</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15.50165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12259,10 +12319,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$156:$Z$156</c:f>
+              <c:f>precision!$B$156:$AE$156</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>0.00189485</c:v>
                 </c:pt>
@@ -12337,6 +12397,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.204612735</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.034515425</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.047525</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.3615</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.916375</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.02025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12353,10 +12428,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$157:$Z$157</c:f>
+              <c:f>precision!$B$157:$AE$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-2.94490905</c:v>
                 </c:pt>
@@ -12431,6 +12506,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.43539168325</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1103033725</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17.67971675</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>17.53525</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20.0774</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>23.1082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12599,10 +12689,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$159:$Z$159</c:f>
+              <c:f>precision!$B$159:$AE$159</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-2.931773225</c:v>
                 </c:pt>
@@ -12677,6 +12767,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.00131615</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.1561739325</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.7007425</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.2223</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.020075</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.769575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12693,10 +12798,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$160:$Z$160</c:f>
+              <c:f>precision!$B$160:$AE$160</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-1.105141325</c:v>
                 </c:pt>
@@ -12771,6 +12876,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-0.33064361725</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1619243625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.096075</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.964775</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.04040000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.33677499999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12787,10 +12907,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$161:$Z$161</c:f>
+              <c:f>precision!$B$161:$AE$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-3.049131975</c:v>
                 </c:pt>
@@ -12865,6 +12985,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-0.95142198975</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.2189968175</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.131885</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21.17885</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22.462225</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21.147725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13033,10 +13168,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$163:$Z$163</c:f>
+              <c:f>precision!$B$163:$AE$163</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-2.108530025</c:v>
                 </c:pt>
@@ -13111,6 +13246,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-7.99322499999999e-05</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.137809605</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.901985</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.5471</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.399275</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.952825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13127,10 +13277,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$164:$Z$164</c:f>
+              <c:f>precision!$B$164:$AE$164</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-1.186992425</c:v>
                 </c:pt>
@@ -13205,6 +13355,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.000231685</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.108126225</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.4629</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.0307</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.40134999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.1724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13221,10 +13386,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>precision!$B$165:$Z$165</c:f>
+              <c:f>precision!$B$165:$AE$165</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-3.06064455</c:v>
                 </c:pt>
@@ -13299,6 +13464,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-0.9971394575</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.9567735525</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17.015605</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18.22715</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22.187</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24.276775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13467,10 +13647,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$151:$Z$151</c:f>
+              <c:f>time!$B$151:$AE$151</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>54.1207269511945</c:v>
                 </c:pt>
@@ -13545,6 +13725,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>99.5162078257718</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.656528225454934</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-26.3421186161085</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-17.6451950110356</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>46.9482480542957</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-10.4414484974897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13561,10 +13756,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$152:$Z$152</c:f>
+              <c:f>time!$B$152:$AE$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>6.06001469921587</c:v>
                 </c:pt>
@@ -13639,6 +13834,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>24.4523619150896</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.30853925218116</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-10.1122360064617</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35.7498144977385</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.25356279462912</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-31.3262911850214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13655,10 +13865,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$153:$Z$153</c:f>
+              <c:f>time!$B$153:$AE$153</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>328.993701072558</c:v>
                 </c:pt>
@@ -13733,6 +13943,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>362.647268402633</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>241.736336599409</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>295.223988019077</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>348.38606302805</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>281.433761378185</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>184.46694296707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13901,10 +14126,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$155:$Z$155</c:f>
+              <c:f>time!$B$155:$AE$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-8.15419571595825</c:v>
                 </c:pt>
@@ -13979,6 +14204,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-5.06004708504616</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.1038655859097</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.93429782512885</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37.4991776439921</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.24984962209956</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18.8561962755451</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13995,10 +14235,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$156:$Z$156</c:f>
+              <c:f>time!$B$156:$AE$156</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-22.5893297493858</c:v>
                 </c:pt>
@@ -14073,6 +14313,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>3.63445404553346</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32.2816762149401</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.7697144656675</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26.5171887701328</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-9.42325274912631</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43.850313242124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14089,10 +14344,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$157:$Z$157</c:f>
+              <c:f>time!$B$157:$AE$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>200.284342383096</c:v>
                 </c:pt>
@@ -14167,6 +14422,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>299.332003243133</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>389.779754661947</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>420.064116951944</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>265.847844026373</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>567.887459934536</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>317.843491937193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14335,10 +14605,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$159:$Z$159</c:f>
+              <c:f>time!$B$159:$AE$159</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-16.2748498537765</c:v>
                 </c:pt>
@@ -14413,6 +14683,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-16.4955301434728</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-39.2105683090051</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-29.1143936149354</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.01729662054272</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.21318043576983</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17.1147349877223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14429,10 +14714,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$160:$Z$160</c:f>
+              <c:f>time!$B$160:$AE$160</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-21.7107535755588</c:v>
                 </c:pt>
@@ -14507,6 +14792,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-33.5384621295512</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-18.5978867121551</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.54077374270742</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.5493831305005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-9.41749867503593</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.6982542502874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14523,10 +14823,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$161:$Z$161</c:f>
+              <c:f>time!$B$161:$AE$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>181.696421148314</c:v>
                 </c:pt>
@@ -14601,6 +14901,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>252.277964286114</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>135.343559661864</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>187.223844061385</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>277.442015480416</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>255.442517114303</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>314.811198546045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14769,10 +15084,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$163:$Z$163</c:f>
+              <c:f>time!$B$163:$AE$163</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>-15.0596551291605</c:v>
                 </c:pt>
@@ -14847,6 +15162,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>47.5363745251829</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16.9591041672136</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-10.4111822600459</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-10.1694156630272</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.64725270951303</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-38.8530008761154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14863,10 +15193,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$164:$Z$164</c:f>
+              <c:f>time!$B$164:$AE$164</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>5.40228990509848</c:v>
                 </c:pt>
@@ -14941,6 +15271,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>27.0130208450776</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-29.8628327049239</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>36.0847933047082</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.90825265554619</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.3793910009885</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-29.000819006557</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14957,10 +15302,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>time!$B$165:$Z$165</c:f>
+              <c:f>time!$B$165:$AE$165</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>137.76819424823</c:v>
                 </c:pt>
@@ -15035,6 +15380,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>243.068686165174</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>296.293965039658</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>411.34367817854</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>254.397105936586</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>153.095289541919</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>113.48963413478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>

</xml_diff>